<commit_message>
Code Additions and Edits
</commit_message>
<xml_diff>
--- a/testData/productItem.xlsx
+++ b/testData/productItem.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="product" sheetId="1" r:id="rId1"/>
     <sheet name="products" sheetId="2" r:id="rId2"/>
+    <sheet name="productItems" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>ProductName</t>
   </si>
@@ -27,13 +28,22 @@
   </si>
   <si>
     <t>Samsung Galaxy A1</t>
+  </si>
+  <si>
+    <t>Airpods</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>Mivi Play 5 Watt Truly Wireless Bluetooth Portable Speaker (Black)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,13 +51,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F1111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,8 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,60 +403,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>